<commit_message>
Update Compliance Testing ZR25.xlsx
Moved Steering knuckle
</commit_message>
<xml_diff>
--- a/MATLAB/compliance_models/Compliance Testing ZR25.xlsx
+++ b/MATLAB/compliance_models/Compliance Testing ZR25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATuck\Documents\GitHub\Vehicle-Dynamics\MATLAB\compliance_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahrn\OneDrive\Documents\Vehicle-Dynamics\MATLAB\compliance_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F2F598-4A97-45BD-B8B1-E633B279BA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316E507E-A510-406D-9918-E537710D8617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{5B56F778-AEBC-4DD0-9364-677FC9B72F2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5B56F778-AEBC-4DD0-9364-677FC9B72F2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -569,27 +569,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE495C62-4CE5-4206-8032-F10ADB68EC30}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="K12" sqref="K12:O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.90625" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17.90625" customWidth="1"/>
-    <col min="6" max="6" width="43.453125" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="43.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -601,7 +601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -633,7 +633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2.5</v>
       </c>
@@ -665,7 +665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>5</v>
       </c>
@@ -697,7 +697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>7.4</v>
       </c>
@@ -729,7 +729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>10</v>
       </c>
@@ -758,7 +758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
@@ -767,7 +767,7 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -784,7 +784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>2.5</v>
       </c>
@@ -801,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>7.3</v>
       </c>
@@ -835,7 +835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -851,96 +851,94 @@
       <c r="E12" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="K12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K14" s="2">
         <v>2.5</v>
       </c>
-      <c r="B15" s="2">
+      <c r="L14" s="2">
         <v>3</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K15" s="2">
         <v>5</v>
       </c>
-      <c r="B16" s="2">
+      <c r="L15" s="2">
         <v>5</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K16" s="2">
         <v>7.3</v>
       </c>
-      <c r="B17" s="2">
+      <c r="L16" s="2">
         <v>7</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K17" s="2">
         <v>10</v>
       </c>
-      <c r="B18" s="2">
+      <c r="L17" s="2">
         <v>12</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I21" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>12</v>
       </c>
@@ -952,7 +950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
@@ -969,7 +967,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>2.5</v>
       </c>
@@ -980,7 +978,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>5</v>
       </c>
@@ -991,7 +989,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>7.6</v>
       </c>
@@ -1002,7 +1000,7 @@
         <v>-37</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>10</v>
       </c>
@@ -1013,7 +1011,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>6</v>
       </c>
@@ -1022,7 +1020,7 @@
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -1033,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>2.5</v>
       </c>
@@ -1044,7 +1042,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>5</v>
       </c>
@@ -1055,7 +1053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>7.3</v>
       </c>
@@ -1066,7 +1064,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -1077,7 +1075,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>8</v>
       </c>
@@ -1086,7 +1084,7 @@
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
@@ -1097,7 +1095,7 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>2.5</v>
       </c>
@@ -1106,7 +1104,7 @@
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>5</v>
       </c>
@@ -1115,7 +1113,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>7.3</v>
       </c>
@@ -1124,7 +1122,7 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>10</v>
       </c>
@@ -1133,14 +1131,14 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1154,7 +1152,7 @@
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="K12:O12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>